<commit_message>
source link about audio
</commit_message>
<xml_diff>
--- a/GUGUENGINE/Submission/poopoopipe_audio/PooPooPiPe_AudioAssetList.xlsx
+++ b/GUGUENGINE/Submission/poopoopipe_audio/PooPooPiPe_AudioAssetList.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMU\Desktop\resubmission\PooPooPipe_audio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\new_99\GUGUENGINE\Submission\poopoopipe_audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1AD289-22A5-4A95-9DAC-07EF55E0A100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A36BD2-FD43-45D5-AEBA-6569593218EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{CB4C77F7-B7D2-4139-A786-672F64E4011D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CB4C77F7-B7D2-4139-A786-672F64E4011D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>TYPE</t>
   </si>
@@ -108,24 +106,127 @@
   </si>
   <si>
     <t>chocob0217@gmail.com</t>
+  </si>
+  <si>
+    <t>fart</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>All Level stage</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>flushing</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>footprint</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>heaven</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>logo</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>siren</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>yeah</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect sound (for prologue cutscene)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect sound (for clear level &amp; prologue cutscene)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect sound (for digipen logo &amp; fmod logo)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect sound (for failing sign &amp; team logo)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect sound (for level5 yellow puzzle explanation)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect sound (every UI in every level)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect sound (for success the level transition)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>prologue cutscene</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>intro</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level5</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://freesound.org/people/shaundoogan/sounds/465486/</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Fewes/sounds/234263/</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Robinhood76/sounds/467441/</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Free-Rush/sounds/472506/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/guitarguy1985/sounds/70938/</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://freesound.org/people/elmasmalo1/sounds/376968/</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://freesound.org/people/simon.rue/sounds/49952/</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -133,22 +234,29 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -310,7 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -344,6 +452,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="강조색6" xfId="1" builtinId="49"/>
@@ -660,23 +770,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F02750-4D03-4053-A6F0-C8A4AF7657B9}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.09765625" customWidth="1"/>
+    <col min="3" max="3" width="31.59765625" customWidth="1"/>
+    <col min="4" max="4" width="29.296875" customWidth="1"/>
     <col min="5" max="5" width="54" customWidth="1"/>
-    <col min="6" max="6" width="102.28515625" customWidth="1"/>
+    <col min="6" max="6" width="102.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.65">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -684,12 +794,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -697,7 +807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -705,7 +815,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -725,7 +835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
@@ -745,7 +855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -765,12 +875,128 @@
         <v>20</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{AEE1EA5F-F8FB-4E65-B794-0E3206A57BD5}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{67110A2E-568B-4904-A93B-8AB6417E91B6}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{258DA234-D4CE-489F-8AF6-89AB342877FD}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{AD0A0BAB-34F4-4B09-969E-6E96641A23E5}"/>
+    <hyperlink ref="E12" r:id="rId5" xr:uid="{753C0CA4-1108-4CDE-8236-3B0647E9F881}"/>
+    <hyperlink ref="E14" r:id="rId6" xr:uid="{501C8398-B74E-4567-81E1-F0C21F8F6333}"/>
+    <hyperlink ref="E15" r:id="rId7" xr:uid="{4177677C-D94B-4285-8A4F-E7963BD3F532}"/>
+    <hyperlink ref="E16" r:id="rId8" xr:uid="{33E41E1C-72B2-4222-B48C-212599A0BFA7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change heaven sound because it was c by nc
</commit_message>
<xml_diff>
--- a/GUGUENGINE/Submission/poopoopipe_audio/PooPooPiPe_AudioAssetList.xlsx
+++ b/GUGUENGINE/Submission/poopoopipe_audio/PooPooPiPe_AudioAssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\new_99\GUGUENGINE\Submission\poopoopipe_audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEC9B1D-1F1C-488B-806B-6C2593A69B7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF545FB2-B81F-49E3-A483-787FB473A58C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CB4C77F7-B7D2-4139-A786-672F64E4011D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
   <si>
     <t>TYPE</t>
   </si>
@@ -189,10 +189,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>https://freesound.org/people/Robinhood76/sounds/467441/</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>https://freesound.org/people/guitarguy1985/sounds/70938/</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -225,10 +221,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Robinhood76</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Free-Rush</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -253,10 +245,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>CC BY-NC 3.0(Attribution-NonCommercial 3.0 Unported, free to share and adapt)/ https://creativecommons.org/licenses/by-nc/3.0/</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>https://freesound.org/people/Free-Rush/sounds/472506/</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -345,6 +333,14 @@
   </si>
   <si>
     <t>CC BY 3.0(Attribution 3.0 Unported, free to share and adapt)/ https://creativecommons.org/licenses/by/3.0/</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://freesound.org/people/random_intruder/sounds/392172/</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>random_intruder</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -910,7 +906,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -933,7 +929,7 @@
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -1023,13 +1019,13 @@
         <v>25</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>43</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -1043,13 +1039,13 @@
         <v>25</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -1063,13 +1059,13 @@
         <v>40</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
@@ -1083,13 +1079,13 @@
         <v>40</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
@@ -1103,13 +1099,13 @@
         <v>41</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
@@ -1123,13 +1119,13 @@
         <v>42</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
@@ -1143,13 +1139,13 @@
         <v>25</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
@@ -1163,93 +1159,93 @@
         <v>25</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
         <v>63</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>69</v>
-      </c>
       <c r="D17" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>70</v>
-      </c>
       <c r="D18" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
         <v>65</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>71</v>
-      </c>
       <c r="D19" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="F20" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>